<commit_message>
[UPDATE] Cambio extraño en el excel :v
</commit_message>
<xml_diff>
--- a/ANEXOS/EntendiendoModelo.xlsx
+++ b/ANEXOS/EntendiendoModelo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d97dfd61da619a5/UNAL FORE/SEMESTRE 9/TECNICAS DE CONTROL/Tareas/T1/aircraft-robust-control-model/ANEXOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3422F86B-4270-47BD-95AD-64463A2EDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B356AC0F-F5BD-47E1-8ED6-C249996C3173}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{3422F86B-4270-47BD-95AD-64463A2EDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35CC7204-C56D-4C4F-847C-B136EB4011C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A4442C4-AD5F-42F6-8E7E-6D1C20D8E6A0}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{1A4442C4-AD5F-42F6-8E7E-6D1C20D8E6A0}"/>
   </bookViews>
   <sheets>
     <sheet name="LinMod" sheetId="2" r:id="rId1"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,16 +266,18 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{99BF7610-59ED-4ADD-AD70-3738E29C6AA3}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,20 +599,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -830,7 +832,7 @@
       </c>
     </row>
     <row r="24" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F24" s="2"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -858,20 +860,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="F3" t="s">
@@ -975,20 +977,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="F3" t="s">

</xml_diff>